<commit_message>
feat: Added bridge tables (Manually)
</commit_message>
<xml_diff>
--- a/assets/pizza_processed.xlsx
+++ b/assets/pizza_processed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caiopavesi/Code/example-etl-pme/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494824C2-80CF-FB4E-AEC8-575390D6355B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0632C8-4707-4443-9C5F-4C62625AAE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Answers" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,29 @@
     <sheet name="Rankings" sheetId="5" r:id="rId5"/>
     <sheet name="AnswersMatrix" sheetId="6" r:id="rId6"/>
     <sheet name="Matrix" sheetId="7" r:id="rId7"/>
-    <sheet name="Categories" sheetId="8" r:id="rId8"/>
+    <sheet name="MatrixStatements" sheetId="9" r:id="rId8"/>
+    <sheet name="MatrixAnswers" sheetId="10" r:id="rId9"/>
+    <sheet name="Categories" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -636,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -4506,6 +4521,41 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE33498-B7BD-BB47-9DD8-4A5C948C02EE}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B211"/>
@@ -14103,8 +14153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14350,33 +14400,89 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE33498-B7BD-BB47-9DD8-4A5C948C02EE}">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2B5422-6000-C644-AC47-292E2EA0ABB2}">
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D315B4-78E4-494D-ACCF-526ED547EE6E}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>